<commit_message>
Added Jacob Graphics and logics
</commit_message>
<xml_diff>
--- a/tony stakov classification/Customer_DATA.xlsx
+++ b/tony stakov classification/Customer_DATA.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinke\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asadtariq/Downloads/Python_work/Python_work/tony stakov classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8DDFE2-6386-4870-887E-41F3206728EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ABD4BE-2F84-624A-890F-31A6DA313177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Φύλλο3" sheetId="4" r:id="rId1"/>
-    <sheet name="Worksheet" sheetId="3" r:id="rId2"/>
+    <sheet name="Worksheet" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1458,7 +1457,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Κανονικό 2" xfId="1" xr:uid="{C4308373-117E-4D0E-9256-6AA8255F614F}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1760,31 +1759,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF59D0B-A18D-4C10-A510-0E2CD6F9CC0F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EFC9AC-3749-488D-A519-822406F73A38}">
   <dimension ref="A1:J504"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M446" sqref="M446"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1816,7 +1803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1848,7 +1835,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1880,7 +1867,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1912,7 +1899,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1944,7 +1931,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1976,7 +1963,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2005,7 +1992,7 @@
         <v>38.9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2037,7 +2024,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2069,7 +2056,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2098,7 +2085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2130,7 +2117,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2162,7 +2149,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2191,7 +2178,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2223,7 +2210,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2252,7 +2239,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2284,7 +2271,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2313,7 +2300,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2345,7 +2332,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2377,7 +2364,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2406,7 +2393,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2435,7 +2422,7 @@
         <v>27.2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2467,7 +2454,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2499,7 +2486,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2531,7 +2518,7 @@
         <v>14.8</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2563,7 +2550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2595,7 +2582,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2624,7 +2611,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2656,7 +2643,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2685,7 +2672,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2717,7 +2704,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2749,7 +2736,7 @@
         <v>7.3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2781,7 +2768,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2813,7 +2800,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2845,7 +2832,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2874,7 +2861,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2906,7 +2893,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2935,7 +2922,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2967,7 +2954,7 @@
         <v>32.700000000000003</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2999,7 +2986,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3031,7 +3018,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3060,7 +3047,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3092,7 +3079,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3124,7 +3111,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3156,7 +3143,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3188,7 +3175,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3220,7 +3207,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3249,7 +3236,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3281,7 +3268,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3310,7 +3297,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3342,7 +3329,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3371,7 +3358,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3403,7 +3390,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3435,7 +3422,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3467,7 +3454,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3496,7 +3483,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3528,7 +3515,7 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -3560,7 +3547,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3592,7 +3579,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -3624,7 +3611,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3656,7 +3643,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -3688,7 +3675,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -3720,7 +3707,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3752,7 +3739,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -3784,7 +3771,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -3816,7 +3803,7 @@
         <v>14.6</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -3848,7 +3835,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -3880,7 +3867,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -3912,7 +3899,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -3944,7 +3931,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -3976,7 +3963,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4008,7 +3995,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4040,7 +4027,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4072,7 +4059,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4104,7 +4091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4133,7 +4120,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4165,7 +4152,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -4197,7 +4184,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -4229,7 +4216,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -4261,7 +4248,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -4293,7 +4280,7 @@
         <v>29.1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -4322,7 +4309,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -4354,7 +4341,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -4386,7 +4373,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -4418,7 +4405,7 @@
         <v>23.3</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -4447,7 +4434,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -4479,7 +4466,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -4508,7 +4495,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -4537,7 +4524,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -4566,7 +4553,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -4598,7 +4585,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -4630,7 +4617,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -4662,7 +4649,7 @@
         <v>26.9</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -4694,7 +4681,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -4726,7 +4713,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -4758,7 +4745,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -4790,7 +4777,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -4819,7 +4806,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -4848,7 +4835,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -4880,7 +4867,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -4912,7 +4899,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -4944,7 +4931,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -4976,7 +4963,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -5005,7 +4992,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -5037,7 +5024,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -5069,7 +5056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -5101,7 +5088,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -5133,7 +5120,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -5165,7 +5152,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -5197,7 +5184,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -5226,7 +5213,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -5258,7 +5245,7 @@
         <v>39.1</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -5290,7 +5277,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -5322,7 +5309,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -5354,7 +5341,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -5386,7 +5373,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -5415,7 +5402,7 @@
         <v>16.8</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -5447,7 +5434,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -5479,7 +5466,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -5508,7 +5495,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -5540,7 +5527,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -5572,7 +5559,7 @@
         <v>10.6</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -5604,7 +5591,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -5636,7 +5623,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -5668,7 +5655,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -5700,7 +5687,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -5732,7 +5719,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -5761,7 +5748,7 @@
         <v>5.9</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -5793,7 +5780,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -5825,7 +5812,7 @@
         <v>10.3</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -5857,7 +5844,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -5889,7 +5876,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -5921,7 +5908,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -5953,7 +5940,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -5985,7 +5972,7 @@
         <v>10.1</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -6017,7 +6004,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -6049,7 +6036,7 @@
         <v>24.7</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -6081,7 +6068,7 @@
         <v>38.200000000000003</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -6110,7 +6097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -6139,7 +6126,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -6171,7 +6158,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -6203,7 +6190,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -6235,7 +6222,7 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -6267,7 +6254,7 @@
         <v>29.1</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -6299,7 +6286,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -6331,7 +6318,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -6363,7 +6350,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -6395,7 +6382,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -6424,7 +6411,7 @@
         <v>11.1</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -6456,7 +6443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -6488,7 +6475,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -6520,7 +6507,7 @@
         <v>26.5</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -6552,7 +6539,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -6581,7 +6568,7 @@
         <v>17.7</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -6613,7 +6600,7 @@
         <v>25.2</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -6642,7 +6629,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -6674,7 +6661,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -6703,7 +6690,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -6735,7 +6722,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -6767,7 +6754,7 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -6799,7 +6786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -6831,7 +6818,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -6860,7 +6847,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -6892,7 +6879,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -6924,7 +6911,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -6956,7 +6943,7 @@
         <v>34.6</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -6988,7 +6975,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -7020,7 +7007,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -7052,7 +7039,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -7084,7 +7071,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -7116,7 +7103,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -7148,7 +7135,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -7180,7 +7167,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -7212,7 +7199,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -7244,7 +7231,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -7276,7 +7263,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -7308,7 +7295,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -7340,7 +7327,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -7372,7 +7359,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -7404,7 +7391,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -7436,7 +7423,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -7468,7 +7455,7 @@
         <v>12.8</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -7500,7 +7487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -7532,7 +7519,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -7564,7 +7551,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -7596,7 +7583,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -7628,7 +7615,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -7660,7 +7647,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -7692,7 +7679,7 @@
         <v>38.200000000000003</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -7724,7 +7711,7 @@
         <v>37.200000000000003</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -7753,7 +7740,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -7782,7 +7769,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -7811,7 +7798,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -7843,7 +7830,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -7872,7 +7859,7 @@
         <v>39.200000000000003</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -7904,7 +7891,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -7936,7 +7923,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -7965,7 +7952,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -7997,7 +7984,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -8029,7 +8016,7 @@
         <v>8.6999999999999993</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -8061,7 +8048,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -8093,7 +8080,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -8125,7 +8112,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -8154,7 +8141,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -8186,7 +8173,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -8218,7 +8205,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -8247,7 +8234,7 @@
         <v>10.199999999999999</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -8279,7 +8266,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -8311,7 +8298,7 @@
         <v>23.6</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -8343,7 +8330,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -8375,7 +8362,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -8407,7 +8394,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -8439,7 +8426,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -8468,7 +8455,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -8500,7 +8487,7 @@
         <v>3.9</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -8529,7 +8516,7 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -8561,7 +8548,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -8593,7 +8580,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -8625,7 +8612,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -8654,7 +8641,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -8683,7 +8670,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -8715,7 +8702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -8747,7 +8734,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -8779,7 +8766,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -8811,7 +8798,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -8843,7 +8830,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -8875,7 +8862,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -8907,7 +8894,7 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -8939,7 +8926,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -8971,7 +8958,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -9003,7 +8990,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -9035,7 +9022,7 @@
         <v>39.6</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>231</v>
       </c>
@@ -9067,7 +9054,7 @@
         <v>37.299999999999997</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>232</v>
       </c>
@@ -9099,7 +9086,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>233</v>
       </c>
@@ -9131,7 +9118,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>234</v>
       </c>
@@ -9160,7 +9147,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>235</v>
       </c>
@@ -9192,7 +9179,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>236</v>
       </c>
@@ -9224,7 +9211,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>237</v>
       </c>
@@ -9253,7 +9240,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>238</v>
       </c>
@@ -9285,7 +9272,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>239</v>
       </c>
@@ -9317,7 +9304,7 @@
         <v>37.9</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>240</v>
       </c>
@@ -9349,7 +9336,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>241</v>
       </c>
@@ -9381,7 +9368,7 @@
         <v>39.700000000000003</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>242</v>
       </c>
@@ -9413,7 +9400,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>243</v>
       </c>
@@ -9442,7 +9429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>244</v>
       </c>
@@ -9474,7 +9461,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>245</v>
       </c>
@@ -9503,7 +9490,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>246</v>
       </c>
@@ -9532,7 +9519,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>247</v>
       </c>
@@ -9564,7 +9551,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>248</v>
       </c>
@@ -9596,7 +9583,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>249</v>
       </c>
@@ -9625,7 +9612,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>250</v>
       </c>
@@ -9657,7 +9644,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>251</v>
       </c>
@@ -9689,7 +9676,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>252</v>
       </c>
@@ -9721,7 +9708,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>253</v>
       </c>
@@ -9753,7 +9740,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>254</v>
       </c>
@@ -9785,7 +9772,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>255</v>
       </c>
@@ -9817,7 +9804,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>256</v>
       </c>
@@ -9849,7 +9836,7 @@
         <v>23.9</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>257</v>
       </c>
@@ -9881,7 +9868,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>258</v>
       </c>
@@ -9913,7 +9900,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>259</v>
       </c>
@@ -9942,7 +9929,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>260</v>
       </c>
@@ -9974,7 +9961,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>261</v>
       </c>
@@ -10006,7 +9993,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>262</v>
       </c>
@@ -10035,7 +10022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>263</v>
       </c>
@@ -10067,7 +10054,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>264</v>
       </c>
@@ -10099,7 +10086,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>265</v>
       </c>
@@ -10131,7 +10118,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>266</v>
       </c>
@@ -10163,7 +10150,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>267</v>
       </c>
@@ -10192,7 +10179,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>268</v>
       </c>
@@ -10224,7 +10211,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>269</v>
       </c>
@@ -10256,7 +10243,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>270</v>
       </c>
@@ -10288,7 +10275,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>271</v>
       </c>
@@ -10320,7 +10307,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>272</v>
       </c>
@@ -10352,7 +10339,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>273</v>
       </c>
@@ -10381,7 +10368,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>274</v>
       </c>
@@ -10410,7 +10397,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>275</v>
       </c>
@@ -10442,7 +10429,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>276</v>
       </c>
@@ -10474,7 +10461,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>277</v>
       </c>
@@ -10506,7 +10493,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>278</v>
       </c>
@@ -10538,7 +10525,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>279</v>
       </c>
@@ -10570,7 +10557,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>280</v>
       </c>
@@ -10602,7 +10589,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>281</v>
       </c>
@@ -10631,7 +10618,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>282</v>
       </c>
@@ -10660,7 +10647,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>283</v>
       </c>
@@ -10692,7 +10679,7 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>284</v>
       </c>
@@ -10724,7 +10711,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>285</v>
       </c>
@@ -10756,7 +10743,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>286</v>
       </c>
@@ -10785,7 +10772,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>287</v>
       </c>
@@ -10817,7 +10804,7 @@
         <v>26.2</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>288</v>
       </c>
@@ -10849,7 +10836,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>289</v>
       </c>
@@ -10881,7 +10868,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>290</v>
       </c>
@@ -10913,7 +10900,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>291</v>
       </c>
@@ -10945,7 +10932,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>292</v>
       </c>
@@ -10974,7 +10961,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>293</v>
       </c>
@@ -11006,7 +10993,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>294</v>
       </c>
@@ -11038,7 +11025,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>295</v>
       </c>
@@ -11070,7 +11057,7 @@
         <v>40.4</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>296</v>
       </c>
@@ -11102,7 +11089,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>297</v>
       </c>
@@ -11134,7 +11121,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>298</v>
       </c>
@@ -11166,7 +11153,7 @@
         <v>10.8</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>299</v>
       </c>
@@ -11198,7 +11185,7 @@
         <v>21.7</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>300</v>
       </c>
@@ -11230,7 +11217,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>301</v>
       </c>
@@ -11262,7 +11249,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>302</v>
       </c>
@@ -11294,7 +11281,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>303</v>
       </c>
@@ -11326,7 +11313,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>304</v>
       </c>
@@ -11358,7 +11345,7 @@
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>305</v>
       </c>
@@ -11390,7 +11377,7 @@
         <v>30.7</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>306</v>
       </c>
@@ -11422,7 +11409,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>307</v>
       </c>
@@ -11454,7 +11441,7 @@
         <v>24.8</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>308</v>
       </c>
@@ -11483,7 +11470,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>309</v>
       </c>
@@ -11515,7 +11502,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>310</v>
       </c>
@@ -11547,7 +11534,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>311</v>
       </c>
@@ -11579,7 +11566,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>312</v>
       </c>
@@ -11611,7 +11598,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>313</v>
       </c>
@@ -11640,7 +11627,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>314</v>
       </c>
@@ -11672,7 +11659,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>315</v>
       </c>
@@ -11704,7 +11691,7 @@
         <v>11.4</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>316</v>
       </c>
@@ -11733,7 +11720,7 @@
         <v>28.3</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>317</v>
       </c>
@@ -11762,7 +11749,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>318</v>
       </c>
@@ -11794,7 +11781,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>319</v>
       </c>
@@ -11823,7 +11810,7 @@
         <v>13.7</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>320</v>
       </c>
@@ -11855,7 +11842,7 @@
         <v>36.1</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>321</v>
       </c>
@@ -11887,7 +11874,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>322</v>
       </c>
@@ -11919,7 +11906,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>323</v>
       </c>
@@ -11951,7 +11938,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>324</v>
       </c>
@@ -11980,7 +11967,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>325</v>
       </c>
@@ -12012,7 +11999,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>326</v>
       </c>
@@ -12044,7 +12031,7 @@
         <v>33.9</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>327</v>
       </c>
@@ -12076,7 +12063,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>328</v>
       </c>
@@ -12108,7 +12095,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>329</v>
       </c>
@@ -12140,7 +12127,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>330</v>
       </c>
@@ -12172,7 +12159,7 @@
         <v>24.3</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>331</v>
       </c>
@@ -12204,7 +12191,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>332</v>
       </c>
@@ -12236,7 +12223,7 @@
         <v>17.8</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>333</v>
       </c>
@@ -12268,7 +12255,7 @@
         <v>30.8</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>334</v>
       </c>
@@ -12300,7 +12287,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>335</v>
       </c>
@@ -12332,7 +12319,7 @@
         <v>14.4</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>336</v>
       </c>
@@ -12364,7 +12351,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>337</v>
       </c>
@@ -12396,7 +12383,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>338</v>
       </c>
@@ -12428,7 +12415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>339</v>
       </c>
@@ -12457,7 +12444,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>340</v>
       </c>
@@ -12489,7 +12476,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>341</v>
       </c>
@@ -12521,7 +12508,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>342</v>
       </c>
@@ -12553,7 +12540,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>343</v>
       </c>
@@ -12582,7 +12569,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>344</v>
       </c>
@@ -12614,7 +12601,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>345</v>
       </c>
@@ -12646,7 +12633,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>346</v>
       </c>
@@ -12678,7 +12665,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>347</v>
       </c>
@@ -12710,7 +12697,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>348</v>
       </c>
@@ -12742,7 +12729,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>349</v>
       </c>
@@ -12774,7 +12761,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>350</v>
       </c>
@@ -12806,7 +12793,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>351</v>
       </c>
@@ -12838,7 +12825,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>352</v>
       </c>
@@ -12870,7 +12857,7 @@
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>353</v>
       </c>
@@ -12902,7 +12889,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>354</v>
       </c>
@@ -12934,7 +12921,7 @@
         <v>28.9</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>355</v>
       </c>
@@ -12966,7 +12953,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>356</v>
       </c>
@@ -12998,7 +12985,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>357</v>
       </c>
@@ -13030,7 +13017,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>358</v>
       </c>
@@ -13062,7 +13049,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>359</v>
       </c>
@@ -13091,7 +13078,7 @@
         <v>9.8000000000000007</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>360</v>
       </c>
@@ -13123,7 +13110,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>361</v>
       </c>
@@ -13155,7 +13142,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>362</v>
       </c>
@@ -13187,7 +13174,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>363</v>
       </c>
@@ -13219,7 +13206,7 @@
         <v>34.700000000000003</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>364</v>
       </c>
@@ -13251,7 +13238,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>365</v>
       </c>
@@ -13283,7 +13270,7 @@
         <v>22.3</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
         <v>366</v>
       </c>
@@ -13315,7 +13302,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>367</v>
       </c>
@@ -13347,7 +13334,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>368</v>
       </c>
@@ -13379,7 +13366,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>369</v>
       </c>
@@ -13411,7 +13398,7 @@
         <v>17.3</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>370</v>
       </c>
@@ -13443,7 +13430,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>371</v>
       </c>
@@ -13475,7 +13462,7 @@
         <v>21.8</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>372</v>
       </c>
@@ -13507,7 +13494,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>373</v>
       </c>
@@ -13539,7 +13526,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>374</v>
       </c>
@@ -13571,7 +13558,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>375</v>
       </c>
@@ -13603,7 +13590,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>376</v>
       </c>
@@ -13635,7 +13622,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>377</v>
       </c>
@@ -13664,7 +13651,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>378</v>
       </c>
@@ -13696,7 +13683,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>379</v>
       </c>
@@ -13728,7 +13715,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>380</v>
       </c>
@@ -13757,7 +13744,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>381</v>
       </c>
@@ -13789,7 +13776,7 @@
         <v>36.799999999999997</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>382</v>
       </c>
@@ -13821,7 +13808,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>383</v>
       </c>
@@ -13853,7 +13840,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>384</v>
       </c>
@@ -13885,7 +13872,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>385</v>
       </c>
@@ -13917,7 +13904,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A387" s="1">
         <v>386</v>
       </c>
@@ -13949,7 +13936,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A388" s="1">
         <v>387</v>
       </c>
@@ -13981,7 +13968,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>388</v>
       </c>
@@ -14013,7 +14000,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A390" s="1">
         <v>389</v>
       </c>
@@ -14045,7 +14032,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A391" s="1">
         <v>390</v>
       </c>
@@ -14077,7 +14064,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A392" s="1">
         <v>391</v>
       </c>
@@ -14109,7 +14096,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A393" s="1">
         <v>392</v>
       </c>
@@ -14141,7 +14128,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A394" s="1">
         <v>393</v>
       </c>
@@ -14173,7 +14160,7 @@
         <v>14.7</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A395" s="1">
         <v>394</v>
       </c>
@@ -14205,7 +14192,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A396" s="1">
         <v>395</v>
       </c>
@@ -14237,7 +14224,7 @@
         <v>6.1</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A397" s="1">
         <v>396</v>
       </c>
@@ -14266,7 +14253,7 @@
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>397</v>
       </c>
@@ -14295,7 +14282,7 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>398</v>
       </c>
@@ -14327,7 +14314,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>399</v>
       </c>
@@ -14359,7 +14346,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A401" s="1">
         <v>400</v>
       </c>
@@ -14388,7 +14375,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A402" s="1">
         <v>401</v>
       </c>
@@ -14420,7 +14407,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A403" s="1">
         <v>402</v>
       </c>
@@ -14452,7 +14439,7 @@
         <v>20.5</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A404" s="1">
         <v>403</v>
       </c>
@@ -14484,7 +14471,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A405" s="1">
         <v>404</v>
       </c>
@@ -14516,7 +14503,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A406" s="1">
         <v>405</v>
       </c>
@@ -14548,7 +14535,7 @@
         <v>31.6</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A407" s="1">
         <v>406</v>
       </c>
@@ -14580,7 +14567,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A408" s="1">
         <v>407</v>
       </c>
@@ -14612,7 +14599,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A409" s="1">
         <v>408</v>
       </c>
@@ -14644,7 +14631,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A410" s="1">
         <v>409</v>
       </c>
@@ -14673,7 +14660,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A411" s="1">
         <v>410</v>
       </c>
@@ -14702,7 +14689,7 @@
         <v>27.7</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A412" s="1">
         <v>411</v>
       </c>
@@ -14734,7 +14721,7 @@
         <v>36.9</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A413" s="1">
         <v>412</v>
       </c>
@@ -14766,7 +14753,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A414" s="1">
         <v>413</v>
       </c>
@@ -14798,7 +14785,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A415" s="1">
         <v>414</v>
       </c>
@@ -14830,7 +14817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A416" s="1">
         <v>415</v>
       </c>
@@ -14862,7 +14849,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A417" s="1">
         <v>416</v>
       </c>
@@ -14894,7 +14881,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A418" s="1">
         <v>417</v>
       </c>
@@ -14923,7 +14910,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A419" s="1">
         <v>418</v>
       </c>
@@ -14955,7 +14942,7 @@
         <v>36.9</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A420" s="1">
         <v>419</v>
       </c>
@@ -14987,7 +14974,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A421" s="1">
         <v>420</v>
       </c>
@@ -15016,7 +15003,7 @@
         <v>30.3</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A422" s="1">
         <v>421</v>
       </c>
@@ -15048,7 +15035,7 @@
         <v>37.1</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A423" s="1">
         <v>422</v>
       </c>
@@ -15080,7 +15067,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A424" s="1">
         <v>423</v>
       </c>
@@ -15109,7 +15096,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A425" s="1">
         <v>424</v>
       </c>
@@ -15141,7 +15128,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A426" s="1">
         <v>425</v>
       </c>
@@ -15170,7 +15157,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A427" s="1">
         <v>426</v>
       </c>
@@ -15202,7 +15189,7 @@
         <v>25.8</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A428" s="1">
         <v>427</v>
       </c>
@@ -15234,7 +15221,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A429" s="1">
         <v>428</v>
       </c>
@@ -15266,7 +15253,7 @@
         <v>18.899999999999999</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A430" s="1">
         <v>429</v>
       </c>
@@ -15298,7 +15285,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
         <v>430</v>
       </c>
@@ -15330,7 +15317,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
         <v>431</v>
       </c>
@@ -15362,7 +15349,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
         <v>432</v>
       </c>
@@ -15391,7 +15378,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
         <v>433</v>
       </c>
@@ -15423,7 +15410,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
         <v>434</v>
       </c>
@@ -15455,7 +15442,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
         <v>435</v>
       </c>
@@ -15487,7 +15474,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
         <v>436</v>
       </c>
@@ -15519,7 +15506,7 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
         <v>437</v>
       </c>
@@ -15551,7 +15538,7 @@
         <v>40.1</v>
       </c>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
         <v>438</v>
       </c>
@@ -15583,7 +15570,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
         <v>439</v>
       </c>
@@ -15615,7 +15602,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
         <v>440</v>
       </c>
@@ -15647,7 +15634,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
         <v>441</v>
       </c>
@@ -15679,7 +15666,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A443" s="1">
         <v>442</v>
       </c>
@@ -15711,7 +15698,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A444" s="1">
         <v>443</v>
       </c>
@@ -15743,7 +15730,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A445" s="1">
         <v>444</v>
       </c>
@@ -15775,7 +15762,7 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A446" s="1">
         <v>445</v>
       </c>
@@ -15804,7 +15791,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A447" s="1">
         <v>446</v>
       </c>
@@ -15836,7 +15823,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A448" s="1">
         <v>447</v>
       </c>
@@ -15868,7 +15855,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A449" s="1">
         <v>448</v>
       </c>
@@ -15900,7 +15887,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="450" spans="1:10" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:10" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A450" s="1">
         <v>449</v>
       </c>
@@ -15932,60 +15919,60 @@
         <v>10.9</v>
       </c>
     </row>
-    <row r="451" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="451" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" spans="1:10" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="13.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>